<commit_message>
minor edits for ChatGPT
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar(1-24-24).xlsx
+++ b/CS320-Spring2024Calendar(1-24-24).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACC354E-9CCF-4A0C-A619-2DE474BE927C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB8DC12-63A0-4F83-9712-8DB25A10A286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52" yWindow="83" windowWidth="28740" windowHeight="15427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="18285" windowHeight="15427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar-Sp24" sheetId="1" r:id="rId1"/>
@@ -319,24 +319,6 @@
 (in-class)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Lecture 2:
-HTML &amp; CSS  w/ChatGPT and self-learning
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 1: HTML &amp; CSS (assigned)</t>
-    </r>
-  </si>
-  <si>
     <t>Lab 1: HTML &amp; CSS  Resume
 due Noon
 (Marmoset)</t>
@@ -446,12 +428,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Lecture 1:
-SW Engineering w/OOP and Agile, 
-Course Calendar, Projects
-</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Course Overview,  Dan Palmieri
 </t>
@@ -516,6 +492,82 @@
 w/Examples
 (Agile Manifesto)
 (Scrum Guide)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lecture 1:
+SW Engineering w/OOP and Agile, 
+Course Calendar, Projects
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Lab 0: Using ChatGPT
+(assigned)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lecture 2:
+HTML &amp; CSS, ChatGPT, and self-learning
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 1: HTML &amp; CSS (assigned)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 0: ChatGPT
+due before class
+(Marmoset)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1217,7 +1269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1468,9 +1520,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1549,50 +1598,95 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1600,94 +1694,34 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1997,10 +2031,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2022,17 +2056,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="146" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
-      <c r="F1" s="112"/>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="113"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="148"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2062,10 +2096,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="116">
+      <c r="A3" s="138">
         <v>15</v>
       </c>
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="133" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="69">
@@ -2097,8 +2131,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="115"/>
-      <c r="B4" s="130"/>
+      <c r="A4" s="142"/>
+      <c r="B4" s="150"/>
       <c r="C4" s="71" t="s">
         <v>7</v>
       </c>
@@ -2119,16 +2153,16 @@
       </c>
       <c r="G4" s="38"/>
       <c r="H4" s="37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I4" s="41"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="115">
+      <c r="A5" s="142">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="135" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="7">
@@ -2159,31 +2193,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="101.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="117"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="157" t="s">
-        <v>73</v>
+    <row r="6" spans="1:18" ht="137.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="139"/>
+      <c r="B6" s="134"/>
+      <c r="C6" s="128" t="s">
+        <v>71</v>
       </c>
       <c r="D6" s="82" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E6" s="59"/>
-      <c r="F6" s="84" t="s">
-        <v>58</v>
+      <c r="F6" s="151" t="s">
+        <v>76</v>
       </c>
       <c r="G6" s="49"/>
-      <c r="H6" s="133" t="s">
+      <c r="H6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="134"/>
+      <c r="I6" s="110"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="118">
+      <c r="A7" s="143">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="122" t="s">
+      <c r="B7" s="131" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="39">
@@ -2216,10 +2250,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="119"/>
-      <c r="B8" s="123"/>
+      <c r="A8" s="136"/>
+      <c r="B8" s="132"/>
       <c r="C8" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="48" t="s">
         <v>32</v>
@@ -2232,16 +2266,16 @@
       <c r="H8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="135" t="s">
+      <c r="I8" s="111" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="119">
+      <c r="A9" s="136">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="123"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2270,18 +2304,18 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
-      <c r="O9" s="148"/>
-      <c r="P9" s="148"/>
-      <c r="Q9" s="148"/>
-      <c r="R9" s="148"/>
+      <c r="L9" s="122"/>
+      <c r="M9" s="122"/>
+      <c r="N9" s="122"/>
+      <c r="O9" s="122"/>
+      <c r="P9" s="122"/>
+      <c r="Q9" s="122"/>
+      <c r="R9" s="122"/>
     </row>
     <row r="10" spans="1:18" ht="80.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="119"/>
-      <c r="B10" s="123"/>
-      <c r="C10" s="136" t="s">
+      <c r="A10" s="136"/>
+      <c r="B10" s="132"/>
+      <c r="C10" s="112" t="s">
         <v>50</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -2293,23 +2327,23 @@
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="L10" s="149"/>
-      <c r="M10" s="148"/>
-      <c r="N10" s="150"/>
-      <c r="O10" s="148"/>
-      <c r="P10" s="150"/>
-      <c r="Q10" s="148"/>
-      <c r="R10" s="150"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="122"/>
+      <c r="N10" s="123"/>
+      <c r="O10" s="122"/>
+      <c r="P10" s="123"/>
+      <c r="Q10" s="122"/>
+      <c r="R10" s="123"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="119">
+      <c r="A11" s="136">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="123"/>
+      <c r="B11" s="132"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2338,17 +2372,17 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="L11" s="148"/>
-      <c r="M11" s="148"/>
-      <c r="N11" s="148"/>
-      <c r="O11" s="148"/>
-      <c r="P11" s="148"/>
-      <c r="Q11" s="148"/>
-      <c r="R11" s="148"/>
+      <c r="L11" s="122"/>
+      <c r="M11" s="122"/>
+      <c r="N11" s="122"/>
+      <c r="O11" s="122"/>
+      <c r="P11" s="122"/>
+      <c r="Q11" s="122"/>
+      <c r="R11" s="122"/>
     </row>
     <row r="12" spans="1:18" ht="90.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="119"/>
-      <c r="B12" s="123"/>
+      <c r="A12" s="136"/>
+      <c r="B12" s="132"/>
       <c r="C12" s="31" t="s">
         <v>45</v>
       </c>
@@ -2364,27 +2398,27 @@
         <v>40</v>
       </c>
       <c r="I12" s="80"/>
-      <c r="L12" s="149"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
-      <c r="O12" s="148"/>
-      <c r="P12" s="150"/>
-      <c r="Q12" s="148"/>
-      <c r="R12" s="150"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="122"/>
+      <c r="N12" s="122"/>
+      <c r="O12" s="122"/>
+      <c r="P12" s="123"/>
+      <c r="Q12" s="122"/>
+      <c r="R12" s="123"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="119">
+      <c r="A13" s="136">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="131" t="s">
+      <c r="B13" s="129" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="17">
         <f>I11 + 1</f>
         <v>25</v>
       </c>
-      <c r="D13" s="86">
+      <c r="D13" s="85">
         <f>C13 + 1</f>
         <v>26</v>
       </c>
@@ -2396,59 +2430,59 @@
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="G13" s="91">
+      <c r="G13" s="90">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="H13" s="76">
         <v>1</v>
       </c>
-      <c r="I13" s="92">
+      <c r="I13" s="91">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L13" s="148"/>
-      <c r="M13" s="148"/>
-      <c r="N13" s="148"/>
-      <c r="O13" s="148"/>
-      <c r="P13" s="148"/>
-      <c r="Q13" s="148"/>
-      <c r="R13" s="151"/>
+      <c r="L13" s="122"/>
+      <c r="M13" s="122"/>
+      <c r="N13" s="122"/>
+      <c r="O13" s="122"/>
+      <c r="P13" s="122"/>
+      <c r="Q13" s="122"/>
+      <c r="R13" s="124"/>
     </row>
     <row r="14" spans="1:18" ht="108.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="124"/>
-      <c r="B14" s="132"/>
+      <c r="A14" s="137"/>
+      <c r="B14" s="130"/>
       <c r="C14" s="29"/>
-      <c r="D14" s="137" t="s">
+      <c r="D14" s="113" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="94"/>
+      <c r="E14" s="93"/>
       <c r="F14" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="88" t="s">
+      <c r="H14" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="89" t="s">
+      <c r="I14" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="L14" s="151"/>
-      <c r="M14" s="149"/>
-      <c r="N14" s="152"/>
-      <c r="O14" s="148"/>
-      <c r="P14" s="151"/>
-      <c r="Q14" s="148"/>
-      <c r="R14" s="151"/>
+      <c r="L14" s="124"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="125"/>
+      <c r="O14" s="122"/>
+      <c r="P14" s="124"/>
+      <c r="Q14" s="122"/>
+      <c r="R14" s="124"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="116">
+      <c r="A15" s="138">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="120" t="s">
+      <c r="B15" s="135" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="69">
@@ -2459,7 +2493,7 @@
         <f t="shared" ref="D15:I15" si="3">C15 + 1</f>
         <v>4</v>
       </c>
-      <c r="E15" s="87">
+      <c r="E15" s="86">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -2467,7 +2501,7 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="G15" s="95">
+      <c r="G15" s="94">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -2475,15 +2509,15 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="I15" s="96">
+      <c r="I15" s="95">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="117"/>
-      <c r="B16" s="121"/>
-      <c r="C16" s="90" t="s">
+      <c r="A16" s="139"/>
+      <c r="B16" s="134"/>
+      <c r="C16" s="89" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -2495,11 +2529,11 @@
       <c r="F16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="97"/>
+      <c r="G16" s="96"/>
       <c r="H16" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="98"/>
+      <c r="I16" s="97"/>
     </row>
     <row r="17" spans="1:18" ht="21.4" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B17" s="24"/>
@@ -2511,686 +2545,665 @@
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
     </row>
-    <row r="19" spans="1:18" s="156" customFormat="1" ht="21" x14ac:dyDescent="0.45">
-      <c r="A19" s="154"/>
-      <c r="B19" s="153"/>
-      <c r="C19" s="153"/>
-      <c r="D19" s="151"/>
-      <c r="E19" s="151"/>
-      <c r="F19" s="151"/>
-      <c r="G19" s="151"/>
-      <c r="H19" s="151"/>
-      <c r="I19" s="155"/>
-    </row>
-    <row r="20" spans="1:18" s="156" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="154"/>
-      <c r="B20" s="153"/>
-      <c r="C20" s="153"/>
-      <c r="D20" s="151"/>
-      <c r="E20" s="151"/>
-      <c r="F20" s="151"/>
-      <c r="G20" s="151"/>
-      <c r="H20" s="151"/>
-      <c r="I20" s="155"/>
-    </row>
-    <row r="21" spans="1:18" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="24"/>
-      <c r="C21" s="35" t="s">
+    <row r="18" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="19" spans="1:18" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="24"/>
+      <c r="C19" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="75" t="s">
+      <c r="D19" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E19" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F19" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="34" t="s">
+      <c r="G19" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="65" t="s">
+      <c r="H19" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="25"/>
-    </row>
-    <row r="22" spans="1:18" s="156" customFormat="1" ht="21.4" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="154"/>
-      <c r="B22" s="153"/>
-      <c r="C22" s="153"/>
-      <c r="D22" s="151"/>
-      <c r="E22" s="151"/>
-      <c r="F22" s="151"/>
-      <c r="G22" s="151"/>
-      <c r="H22" s="151"/>
-      <c r="I22" s="155"/>
-    </row>
-    <row r="23" spans="1:18" s="156" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="154"/>
-      <c r="B23" s="153"/>
-      <c r="C23" s="153"/>
-      <c r="D23" s="151"/>
-      <c r="E23" s="151"/>
-      <c r="F23" s="151"/>
-      <c r="G23" s="151"/>
-      <c r="H23" s="151"/>
-      <c r="I23" s="155"/>
-    </row>
-    <row r="24" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="111" t="str">
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:18" s="127" customFormat="1" ht="21.4" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="126"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="124"/>
+      <c r="E20" s="124"/>
+      <c r="F20" s="124"/>
+      <c r="G20" s="124"/>
+      <c r="H20" s="124"/>
+      <c r="I20" s="124"/>
+    </row>
+    <row r="21" spans="1:18" s="127" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="126"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="124"/>
+      <c r="E21" s="124"/>
+      <c r="F21" s="124"/>
+      <c r="G21" s="124"/>
+      <c r="H21" s="124"/>
+      <c r="I21" s="124"/>
+    </row>
+    <row r="22" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="146" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
 (as of 1-24-2024, subject to change)</v>
       </c>
-      <c r="B24" s="112"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="112"/>
-      <c r="I24" s="113"/>
-    </row>
-    <row r="25" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="1" t="str">
+      <c r="B22" s="147"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="147"/>
+      <c r="E22" s="147"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="147"/>
+      <c r="H22" s="147"/>
+      <c r="I22" s="148"/>
+    </row>
+    <row r="23" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="1" t="str">
         <f>A2</f>
         <v>Weeks</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="str">
-        <f>C2</f>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="str">
+        <f t="shared" ref="C23:I23" si="4">C2</f>
         <v>Sunday</v>
       </c>
-      <c r="D25" s="1" t="str">
-        <f>D2</f>
+      <c r="D23" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Monday</v>
       </c>
-      <c r="E25" s="1" t="str">
-        <f>E2</f>
+      <c r="E23" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Tuesday</v>
       </c>
-      <c r="F25" s="1" t="str">
-        <f>F2</f>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Wednesday</v>
       </c>
-      <c r="G25" s="1" t="str">
-        <f>G2</f>
+      <c r="G23" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Thursday</v>
       </c>
-      <c r="H25" s="1" t="str">
-        <f>H2</f>
+      <c r="H23" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Friday</v>
       </c>
-      <c r="I25" s="1" t="str">
-        <f>I2</f>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="4"/>
         <v>Saturday</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="114">
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="149">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B26" s="120" t="s">
+      <c r="B24" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="99">
+      <c r="C24" s="98">
         <f>I15 + 1</f>
         <v>10</v>
       </c>
+      <c r="D24" s="18">
+        <f>C24 + 1</f>
+        <v>11</v>
+      </c>
+      <c r="E24" s="18">
+        <f t="shared" ref="E24:I24" si="5">D24 + 1</f>
+        <v>12</v>
+      </c>
+      <c r="F24" s="18">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="G24" s="18">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="H24" s="18">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="I24" s="19">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="L24" s="124"/>
+      <c r="M24" s="122"/>
+      <c r="N24" s="122"/>
+      <c r="O24" s="122"/>
+      <c r="P24" s="122"/>
+      <c r="Q24" s="122"/>
+      <c r="R24" s="122"/>
+    </row>
+    <row r="25" spans="1:18" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="142"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="36"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="122"/>
+      <c r="N25" s="122"/>
+      <c r="O25" s="122"/>
+      <c r="P25" s="122"/>
+      <c r="Q25" s="122"/>
+      <c r="R25" s="25"/>
+    </row>
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="142">
+        <f>A24 - 1</f>
+        <v>7</v>
+      </c>
+      <c r="B26" s="135"/>
+      <c r="C26" s="7">
+        <f>I24 + 1</f>
+        <v>17</v>
+      </c>
       <c r="D26" s="18">
         <f>C26 + 1</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E26" s="18">
-        <f t="shared" ref="E26:I26" si="4">D26 + 1</f>
-        <v>12</v>
+        <f t="shared" ref="E26:I26" si="6">D26 + 1</f>
+        <v>19</v>
       </c>
       <c r="F26" s="18">
-        <f t="shared" si="4"/>
-        <v>13</v>
+        <f t="shared" si="6"/>
+        <v>20</v>
       </c>
       <c r="G26" s="18">
-        <f t="shared" si="4"/>
-        <v>14</v>
+        <f t="shared" si="6"/>
+        <v>21</v>
       </c>
       <c r="H26" s="18">
-        <f t="shared" si="4"/>
-        <v>15</v>
+        <f t="shared" si="6"/>
+        <v>22</v>
       </c>
       <c r="I26" s="19">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-      <c r="L26" s="151"/>
-      <c r="M26" s="148"/>
-      <c r="N26" s="148"/>
-      <c r="O26" s="148"/>
-      <c r="P26" s="148"/>
-      <c r="Q26" s="148"/>
-      <c r="R26" s="148"/>
-    </row>
-    <row r="27" spans="1:18" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="115"/>
-      <c r="B27" s="120"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="36"/>
-      <c r="L27" s="149"/>
-      <c r="M27" s="148"/>
-      <c r="N27" s="148"/>
-      <c r="O27" s="148"/>
-      <c r="P27" s="148"/>
-      <c r="Q27" s="148"/>
-      <c r="R27" s="149"/>
+        <f t="shared" si="6"/>
+        <v>23</v>
+      </c>
+      <c r="L26" s="122"/>
+      <c r="M26" s="122"/>
+      <c r="N26" s="122"/>
+      <c r="O26" s="122"/>
+      <c r="P26" s="122"/>
+      <c r="Q26" s="122"/>
+      <c r="R26" s="122"/>
+    </row>
+    <row r="27" spans="1:18" ht="129.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="142"/>
+      <c r="B27" s="135"/>
+      <c r="C27" s="121"/>
+      <c r="D27" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="114" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="114" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27" s="120" t="s">
+        <v>53</v>
+      </c>
+      <c r="L27" s="25"/>
+      <c r="M27" s="122"/>
+      <c r="N27" s="124"/>
+      <c r="O27" s="122"/>
+      <c r="P27" s="124"/>
+      <c r="Q27" s="122"/>
+      <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="115">
+      <c r="A28" s="142">
         <f>A26 - 1</f>
-        <v>7</v>
-      </c>
-      <c r="B28" s="120"/>
+        <v>6</v>
+      </c>
+      <c r="B28" s="135"/>
       <c r="C28" s="7">
         <f>I26 + 1</f>
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D28" s="18">
         <f>C28 + 1</f>
-        <v>18</v>
-      </c>
-      <c r="E28" s="18">
-        <f t="shared" ref="E28:I28" si="5">D28 + 1</f>
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" ref="E28:G30" si="7">D28 + 1</f>
+        <v>26</v>
       </c>
       <c r="F28" s="18">
-        <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="G28" s="18">
-        <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
-      <c r="H28" s="18">
-        <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="I28" s="19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
+        <v>27</v>
+      </c>
+      <c r="G28" s="84">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+      <c r="H28" s="104">
+        <f t="shared" ref="H28" si="8">G28 + 1</f>
+        <v>29</v>
+      </c>
+      <c r="I28" s="90">
+        <f t="shared" ref="I28" si="9">H28 + 1</f>
+        <v>30</v>
+      </c>
+      <c r="L28" s="122"/>
+      <c r="M28" s="122"/>
+      <c r="N28" s="122"/>
+      <c r="O28" s="122"/>
+      <c r="P28" s="122"/>
+      <c r="Q28" s="122"/>
+      <c r="R28" s="122"/>
+    </row>
+    <row r="29" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A29" s="139"/>
+      <c r="B29" s="134"/>
+      <c r="C29" s="115"/>
+      <c r="D29" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="L28" s="148"/>
-      <c r="M28" s="148"/>
-      <c r="N28" s="148"/>
-      <c r="O28" s="148"/>
-      <c r="P28" s="148"/>
-      <c r="Q28" s="148"/>
-      <c r="R28" s="148"/>
-    </row>
-    <row r="29" spans="1:18" ht="129.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="115"/>
-      <c r="B29" s="120"/>
-      <c r="C29" s="147"/>
-      <c r="D29" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="138" t="s">
-        <v>69</v>
-      </c>
-      <c r="F29" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="138" t="s">
-        <v>52</v>
-      </c>
-      <c r="H29" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="I29" s="146" t="s">
-        <v>53</v>
-      </c>
-      <c r="L29" s="149"/>
-      <c r="M29" s="148"/>
-      <c r="N29" s="151"/>
-      <c r="O29" s="148"/>
-      <c r="P29" s="151"/>
-      <c r="Q29" s="148"/>
-      <c r="R29" s="149"/>
-    </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="115">
-        <f>A28 - 1</f>
+      <c r="E29" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="99"/>
+      <c r="H29" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="119" t="s">
+        <v>48</v>
+      </c>
+      <c r="L29" s="25"/>
+      <c r="M29" s="122"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="122"/>
+      <c r="P29" s="25"/>
+      <c r="Q29" s="124"/>
+      <c r="R29" s="25"/>
+    </row>
+    <row r="30" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="143">
+        <f>A28 -1</f>
+        <v>5</v>
+      </c>
+      <c r="B30" s="131" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="105">
+        <f>I28 + 1</f>
+        <v>31</v>
+      </c>
+      <c r="D30" s="106">
+        <v>1</v>
+      </c>
+      <c r="E30" s="40">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="F30" s="55">
+        <f>E30 + 1</f>
+        <v>3</v>
+      </c>
+      <c r="G30" s="46">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="H30" s="15">
+        <f>G30 + 1</f>
+        <v>5</v>
+      </c>
+      <c r="I30" s="61">
+        <f>H30 + 1</f>
         <v>6</v>
       </c>
-      <c r="B30" s="120"/>
-      <c r="C30" s="7">
-        <f>I28 + 1</f>
-        <v>24</v>
-      </c>
-      <c r="D30" s="18">
-        <f>C30 + 1</f>
-        <v>25</v>
-      </c>
-      <c r="E30" s="6">
-        <f t="shared" ref="E30:G32" si="6">D30 + 1</f>
-        <v>26</v>
-      </c>
-      <c r="F30" s="18">
-        <f t="shared" si="6"/>
-        <v>27</v>
-      </c>
-      <c r="G30" s="85">
-        <f t="shared" si="6"/>
+    </row>
+    <row r="31" spans="1:18" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="144"/>
+      <c r="B31" s="130"/>
+      <c r="C31" s="118" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="27"/>
+      <c r="F31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="81"/>
+      <c r="H31" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" s="28"/>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="145">
+        <f>A30 -1</f>
+        <v>4</v>
+      </c>
+      <c r="B32" s="131" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="62">
+        <f>I30 + 1</f>
+        <v>7</v>
+      </c>
+      <c r="D32" s="46">
+        <f>C32 + 1</f>
+        <v>8</v>
+      </c>
+      <c r="E32" s="15">
+        <f t="shared" ref="E32:I32" si="10">D32 + 1</f>
+        <v>9</v>
+      </c>
+      <c r="F32" s="15">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="G32" s="46">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="H32" s="27">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="I32" s="28">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="136"/>
+      <c r="B33" s="132"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="116" t="s">
         <v>28</v>
       </c>
-      <c r="H30" s="105">
-        <f t="shared" ref="H30" si="7">G30 + 1</f>
-        <v>29</v>
-      </c>
-      <c r="I30" s="91">
-        <f t="shared" ref="I30" si="8">H30 + 1</f>
-        <v>30</v>
-      </c>
-      <c r="L30" s="148"/>
-      <c r="M30" s="148"/>
-      <c r="N30" s="148"/>
-      <c r="O30" s="148"/>
-      <c r="P30" s="148"/>
-      <c r="Q30" s="148"/>
-      <c r="R30" s="148"/>
-    </row>
-    <row r="31" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="117"/>
-      <c r="B31" s="121"/>
-      <c r="C31" s="139"/>
-      <c r="D31" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" s="100"/>
-      <c r="H31" s="74" t="s">
-        <v>48</v>
-      </c>
-      <c r="I31" s="145" t="s">
-        <v>48</v>
-      </c>
-      <c r="L31" s="149"/>
-      <c r="M31" s="148"/>
-      <c r="N31" s="149"/>
-      <c r="O31" s="148"/>
-      <c r="P31" s="149"/>
-      <c r="Q31" s="151"/>
-      <c r="R31" s="149"/>
-    </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="118">
-        <f>A30 -1</f>
-        <v>5</v>
-      </c>
-      <c r="B32" s="122" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="106">
-        <f>I30 + 1</f>
-        <v>31</v>
-      </c>
-      <c r="D32" s="107">
-        <v>1</v>
-      </c>
-      <c r="E32" s="40">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-      <c r="F32" s="55">
-        <f>E32 + 1</f>
-        <v>3</v>
-      </c>
-      <c r="G32" s="46">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="H32" s="15">
-        <f>G32 + 1</f>
-        <v>5</v>
-      </c>
-      <c r="I32" s="61">
-        <f>H32 + 1</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="128"/>
-      <c r="B33" s="132"/>
-      <c r="C33" s="144" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="108" t="s">
-        <v>48</v>
-      </c>
-      <c r="E33" s="27"/>
+      <c r="E33" s="117" t="s">
+        <v>65</v>
+      </c>
       <c r="F33" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G33" s="81"/>
-      <c r="H33" s="12" t="s">
-        <v>60</v>
+      <c r="G33" s="27"/>
+      <c r="H33" s="109" t="s">
+        <v>61</v>
       </c>
       <c r="I33" s="28"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="129">
+    <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="136">
         <f>A32 -1</f>
-        <v>4</v>
-      </c>
-      <c r="B34" s="122" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="62">
+        <v>3</v>
+      </c>
+      <c r="B34" s="132"/>
+      <c r="C34" s="27">
         <f>I32 + 1</f>
-        <v>7</v>
-      </c>
-      <c r="D34" s="46">
+        <v>14</v>
+      </c>
+      <c r="D34" s="27">
         <f>C34 + 1</f>
-        <v>8</v>
-      </c>
-      <c r="E34" s="15">
-        <f t="shared" ref="E34:I34" si="9">D34 + 1</f>
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="E34" s="12">
+        <f t="shared" ref="E34:I34" si="11">D34 + 1</f>
+        <v>16</v>
       </c>
       <c r="F34" s="15">
-        <f t="shared" si="9"/>
-        <v>10</v>
-      </c>
-      <c r="G34" s="46">
-        <f t="shared" si="9"/>
-        <v>11</v>
+        <f t="shared" si="11"/>
+        <v>17</v>
+      </c>
+      <c r="G34" s="27">
+        <f t="shared" si="11"/>
+        <v>18</v>
       </c>
       <c r="H34" s="27">
-        <f t="shared" si="9"/>
-        <v>12</v>
+        <f t="shared" si="11"/>
+        <v>19</v>
       </c>
       <c r="I34" s="28">
-        <f t="shared" si="9"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="119"/>
-      <c r="B35" s="123"/>
+        <f t="shared" si="11"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="136"/>
+      <c r="B35" s="132"/>
       <c r="C35" s="29"/>
-      <c r="D35" s="141" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="142" t="s">
-        <v>66</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="G35" s="27"/>
-      <c r="H35" s="110" t="s">
-        <v>62</v>
+      <c r="D35" s="108" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="81"/>
+      <c r="H35" s="12" t="s">
+        <v>6</v>
       </c>
       <c r="I35" s="28"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="119">
+      <c r="A36" s="136">
         <f>A34 -1</f>
-        <v>3</v>
-      </c>
-      <c r="B36" s="123"/>
-      <c r="C36" s="27">
+        <v>2</v>
+      </c>
+      <c r="B36" s="132"/>
+      <c r="C36" s="29">
         <f>I34 + 1</f>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D36" s="27">
         <f>C36 + 1</f>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E36" s="12">
-        <f t="shared" ref="E36:I36" si="10">D36 + 1</f>
-        <v>16</v>
-      </c>
-      <c r="F36" s="15">
-        <f t="shared" si="10"/>
-        <v>17</v>
-      </c>
-      <c r="G36" s="27">
-        <f t="shared" si="10"/>
-        <v>18</v>
-      </c>
-      <c r="H36" s="27">
-        <f t="shared" si="10"/>
-        <v>19</v>
-      </c>
-      <c r="I36" s="28">
-        <f t="shared" si="10"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="119"/>
-      <c r="B37" s="123"/>
-      <c r="C37" s="143"/>
-      <c r="D37" s="109" t="s">
+        <f t="shared" ref="E36:I38" si="12">D36 + 1</f>
+        <v>23</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="12"/>
+        <v>24</v>
+      </c>
+      <c r="G36" s="12">
+        <f t="shared" si="12"/>
+        <v>25</v>
+      </c>
+      <c r="H36" s="12">
+        <f t="shared" si="12"/>
+        <v>26</v>
+      </c>
+      <c r="I36" s="16">
+        <f t="shared" si="12"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A37" s="137"/>
+      <c r="B37" s="130"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="43"/>
+      <c r="F37" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="140" t="s">
+      <c r="G37" s="43"/>
+      <c r="H37" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="81"/>
-      <c r="H37" s="133" t="s">
+      <c r="I37" s="42"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="138">
+        <f>A36 -1</f>
+        <v>1</v>
+      </c>
+      <c r="B38" s="133" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="17">
+        <f>I36 + 1</f>
+        <v>28</v>
+      </c>
+      <c r="D38" s="12">
+        <f>C38 + 1</f>
+        <v>29</v>
+      </c>
+      <c r="E38" s="16">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="F38" s="100">
+        <v>1</v>
+      </c>
+      <c r="G38" s="4">
+        <f>F38 + 1</f>
+        <v>2</v>
+      </c>
+      <c r="H38" s="4">
+        <f>G38 + 1</f>
+        <v>3</v>
+      </c>
+      <c r="I38" s="5">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A39" s="139"/>
+      <c r="B39" s="134"/>
+      <c r="C39" s="102"/>
+      <c r="D39" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="I37" s="28"/>
-    </row>
-    <row r="38" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="119">
-        <f>A36 -1</f>
-        <v>2</v>
-      </c>
-      <c r="B38" s="123"/>
-      <c r="C38" s="29">
-        <f>I36 + 1</f>
-        <v>21</v>
-      </c>
-      <c r="D38" s="27">
-        <f>C38 + 1</f>
-        <v>22</v>
-      </c>
-      <c r="E38" s="12">
-        <f t="shared" ref="E38:I40" si="11">D38 + 1</f>
-        <v>23</v>
-      </c>
-      <c r="F38" s="12">
-        <f t="shared" si="11"/>
-        <v>24</v>
-      </c>
-      <c r="G38" s="12">
-        <f t="shared" si="11"/>
-        <v>25</v>
-      </c>
-      <c r="H38" s="12">
-        <f t="shared" si="11"/>
-        <v>26</v>
-      </c>
-      <c r="I38" s="16">
-        <f t="shared" si="11"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="124"/>
-      <c r="B39" s="132"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="E39" s="43"/>
-      <c r="F39" s="45" t="s">
+      <c r="E39" s="103"/>
+      <c r="F39" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="G39" s="43"/>
-      <c r="H39" s="45" t="s">
+      <c r="G39" s="6"/>
+      <c r="H39" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I39" s="30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="140" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="20">
+        <f>I38 + 1</f>
+        <v>5</v>
+      </c>
+      <c r="D40" s="18">
+        <f t="shared" ref="D40:I40" si="13">C40 + 1</f>
         <v>6</v>
       </c>
-      <c r="I39" s="42"/>
-    </row>
-    <row r="40" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="116">
-        <f>A38 -1</f>
-        <v>1</v>
-      </c>
-      <c r="B40" s="125" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="17">
-        <f>I38 + 1</f>
-        <v>28</v>
-      </c>
-      <c r="D40" s="12">
-        <f>C40 + 1</f>
-        <v>29</v>
-      </c>
-      <c r="E40" s="16">
-        <f t="shared" si="11"/>
-        <v>30</v>
-      </c>
-      <c r="F40" s="101">
-        <v>1</v>
-      </c>
-      <c r="G40" s="4">
-        <f>F40 + 1</f>
-        <v>2</v>
-      </c>
-      <c r="H40" s="4">
-        <f>G40 + 1</f>
-        <v>3</v>
-      </c>
-      <c r="I40" s="5">
-        <f t="shared" si="11"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="117"/>
-      <c r="B41" s="121"/>
-      <c r="C41" s="103"/>
-      <c r="D41" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="104"/>
-      <c r="F41" s="102" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I41" s="30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="126" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="120" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="20">
-        <f>I40 + 1</f>
-        <v>5</v>
-      </c>
-      <c r="D42" s="18">
-        <f t="shared" ref="D42:I42" si="12">C42 + 1</f>
-        <v>6</v>
-      </c>
-      <c r="E42" s="58">
-        <f t="shared" si="12"/>
+      <c r="E40" s="58">
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="F42" s="18">
-        <f t="shared" si="12"/>
+      <c r="F40" s="18">
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
-      <c r="G42" s="18">
-        <f t="shared" si="12"/>
+      <c r="G40" s="18">
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
-      <c r="H42" s="76">
-        <f t="shared" si="12"/>
+      <c r="H40" s="76">
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="I42" s="77">
-        <f t="shared" si="12"/>
+      <c r="I40" s="77">
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="127"/>
-      <c r="B43" s="121"/>
-      <c r="C43" s="63" t="s">
+    <row r="41" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A41" s="141"/>
+      <c r="B41" s="134"/>
+      <c r="C41" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D41" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="64"/>
+      <c r="F41" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="64"/>
-      <c r="F43" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="G43" s="21"/>
-      <c r="H43" s="78"/>
-      <c r="I43" s="79"/>
-    </row>
-    <row r="44" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="78"/>
+      <c r="I41" s="79"/>
+    </row>
+    <row r="42" spans="1:9" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A36:A37"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A24:A25"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A22:I22"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="B24:B29"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B41"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>

</xml_diff>

<commit_message>
edits for moving labs
</commit_message>
<xml_diff>
--- a/CS320-Spring2024Calendar(1-24-24).xlsx
+++ b/CS320-Spring2024Calendar(1-24-24).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\donha\cs320-spring2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB8DC12-63A0-4F83-9712-8DB25A10A286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA119ED1-1776-4C33-A3E8-91FBF0A5E0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="735" yWindow="735" windowWidth="18285" windowHeight="15427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
   <si>
     <t>Monday</t>
   </si>
@@ -240,12 +240,6 @@
   </si>
   <si>
     <t>May/Apr</t>
-  </si>
-  <si>
-    <t>Lab 2a: Web
-Applications
-due Noon
-(Marmoset)</t>
   </si>
   <si>
     <t>Intro to Relational Databases, SQL, JDBC, ORM Labs</t>
@@ -568,6 +562,12 @@
 due before class
 (Marmoset)</t>
     </r>
+  </si>
+  <si>
+    <t>Lab 2a: Web
+Applications
+due Noon (after sign-off)
+(Marmoset)</t>
   </si>
 </sst>
 </file>
@@ -1269,7 +1269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1622,9 +1622,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1722,6 +1719,15 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2033,8 +2039,8 @@
   </sheetPr>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2056,17 +2062,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="53.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="146" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
-      <c r="D1" s="147"/>
-      <c r="E1" s="147"/>
-      <c r="F1" s="147"/>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="148"/>
+      <c r="A1" s="145" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="147"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -2096,10 +2102,10 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="138">
+      <c r="A3" s="137">
         <v>15</v>
       </c>
-      <c r="B3" s="133" t="s">
+      <c r="B3" s="132" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="69">
@@ -2131,8 +2137,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="142"/>
-      <c r="B4" s="150"/>
+      <c r="A4" s="141"/>
+      <c r="B4" s="149"/>
       <c r="C4" s="71" t="s">
         <v>7</v>
       </c>
@@ -2153,16 +2159,16 @@
       </c>
       <c r="G4" s="38"/>
       <c r="H4" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" s="41"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="142">
+      <c r="A5" s="141">
         <f>A3 - 1</f>
         <v>14</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="134" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="7">
@@ -2194,17 +2200,17 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="137.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="139"/>
-      <c r="B6" s="134"/>
-      <c r="C6" s="128" t="s">
-        <v>71</v>
+      <c r="A6" s="138"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="127" t="s">
+        <v>70</v>
       </c>
       <c r="D6" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="59"/>
+      <c r="F6" s="150" t="s">
         <v>75</v>
-      </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="151" t="s">
-        <v>76</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="12" t="s">
@@ -2213,11 +2219,11 @@
       <c r="I6" s="110"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="143">
+      <c r="A7" s="142">
         <f>A5 - 1</f>
         <v>13</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="130" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="39">
@@ -2250,10 +2256,10 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="87.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="136"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="135"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="48" t="s">
         <v>32</v>
@@ -2267,15 +2273,15 @@
         <v>31</v>
       </c>
       <c r="I8" s="111" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="136">
+      <c r="A9" s="135">
         <f>A7 - 1</f>
         <v>12</v>
       </c>
-      <c r="B9" s="132"/>
+      <c r="B9" s="131"/>
       <c r="C9" s="14">
         <f>I7 + 1</f>
         <v>11</v>
@@ -2304,22 +2310,22 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="L9" s="122"/>
-      <c r="M9" s="122"/>
-      <c r="N9" s="122"/>
-      <c r="O9" s="122"/>
-      <c r="P9" s="122"/>
-      <c r="Q9" s="122"/>
-      <c r="R9" s="122"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="121"/>
+      <c r="R9" s="121"/>
     </row>
     <row r="10" spans="1:18" ht="80.650000000000006" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="136"/>
-      <c r="B10" s="132"/>
+      <c r="A10" s="135"/>
+      <c r="B10" s="131"/>
       <c r="C10" s="112" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="10" t="s">
@@ -2327,23 +2333,23 @@
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I10" s="13"/>
       <c r="L10" s="25"/>
-      <c r="M10" s="122"/>
-      <c r="N10" s="123"/>
-      <c r="O10" s="122"/>
-      <c r="P10" s="123"/>
-      <c r="Q10" s="122"/>
-      <c r="R10" s="123"/>
+      <c r="M10" s="121"/>
+      <c r="N10" s="122"/>
+      <c r="O10" s="121"/>
+      <c r="P10" s="122"/>
+      <c r="Q10" s="121"/>
+      <c r="R10" s="122"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="136">
+      <c r="A11" s="135">
         <f>A9 -1</f>
         <v>11</v>
       </c>
-      <c r="B11" s="132"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="17">
         <f>I9 + 1</f>
         <v>18</v>
@@ -2372,24 +2378,24 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="L11" s="122"/>
-      <c r="M11" s="122"/>
-      <c r="N11" s="122"/>
-      <c r="O11" s="122"/>
-      <c r="P11" s="122"/>
-      <c r="Q11" s="122"/>
-      <c r="R11" s="122"/>
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="121"/>
+      <c r="O11" s="121"/>
+      <c r="P11" s="121"/>
+      <c r="Q11" s="121"/>
+      <c r="R11" s="121"/>
     </row>
     <row r="12" spans="1:18" ht="90.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="136"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="31" t="s">
-        <v>45</v>
-      </c>
+      <c r="A12" s="135"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="152"/>
       <c r="D12" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="151" t="s">
+        <v>76</v>
+      </c>
       <c r="F12" s="45" t="s">
         <v>39</v>
       </c>
@@ -2399,19 +2405,19 @@
       </c>
       <c r="I12" s="80"/>
       <c r="L12" s="25"/>
-      <c r="M12" s="122"/>
-      <c r="N12" s="122"/>
-      <c r="O12" s="122"/>
-      <c r="P12" s="123"/>
-      <c r="Q12" s="122"/>
-      <c r="R12" s="123"/>
+      <c r="M12" s="121"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="121"/>
+      <c r="P12" s="122"/>
+      <c r="Q12" s="121"/>
+      <c r="R12" s="122"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="136">
+      <c r="A13" s="135">
         <f xml:space="preserve"> A11 - 1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="129" t="s">
+      <c r="B13" s="128" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="17">
@@ -2441,24 +2447,24 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="L13" s="122"/>
-      <c r="M13" s="122"/>
-      <c r="N13" s="122"/>
-      <c r="O13" s="122"/>
-      <c r="P13" s="122"/>
-      <c r="Q13" s="122"/>
-      <c r="R13" s="124"/>
+      <c r="L13" s="121"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="121"/>
+      <c r="P13" s="121"/>
+      <c r="Q13" s="121"/>
+      <c r="R13" s="123"/>
     </row>
     <row r="14" spans="1:18" ht="108.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="137"/>
-      <c r="B14" s="130"/>
+      <c r="A14" s="136"/>
+      <c r="B14" s="129"/>
       <c r="C14" s="29"/>
       <c r="D14" s="113" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="93"/>
       <c r="F14" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G14" s="92" t="s">
         <v>42</v>
@@ -2469,20 +2475,20 @@
       <c r="I14" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="L14" s="124"/>
+      <c r="L14" s="123"/>
       <c r="M14" s="25"/>
-      <c r="N14" s="125"/>
-      <c r="O14" s="122"/>
-      <c r="P14" s="124"/>
-      <c r="Q14" s="122"/>
-      <c r="R14" s="124"/>
+      <c r="N14" s="124"/>
+      <c r="O14" s="121"/>
+      <c r="P14" s="123"/>
+      <c r="Q14" s="121"/>
+      <c r="R14" s="123"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="138">
+      <c r="A15" s="137">
         <f>A13 - 1</f>
         <v>9</v>
       </c>
-      <c r="B15" s="135" t="s">
+      <c r="B15" s="134" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="69">
@@ -2515,23 +2521,23 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="139"/>
-      <c r="B16" s="134"/>
+      <c r="A16" s="138"/>
+      <c r="B16" s="133"/>
       <c r="C16" s="89" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G16" s="96"/>
       <c r="H16" s="66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" s="97"/>
     </row>
@@ -2568,42 +2574,42 @@
       </c>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="1:18" s="127" customFormat="1" ht="21.4" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="126"/>
+    <row r="20" spans="1:18" s="126" customFormat="1" ht="21.4" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="125"/>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="124"/>
-      <c r="H20" s="124"/>
-      <c r="I20" s="124"/>
-    </row>
-    <row r="21" spans="1:18" s="127" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="126"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="123"/>
+      <c r="F20" s="123"/>
+      <c r="G20" s="123"/>
+      <c r="H20" s="123"/>
+      <c r="I20" s="123"/>
+    </row>
+    <row r="21" spans="1:18" s="126" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="125"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35"/>
-      <c r="D21" s="124"/>
-      <c r="E21" s="124"/>
-      <c r="F21" s="124"/>
-      <c r="G21" s="124"/>
-      <c r="H21" s="124"/>
-      <c r="I21" s="124"/>
+      <c r="D21" s="123"/>
+      <c r="E21" s="123"/>
+      <c r="F21" s="123"/>
+      <c r="G21" s="123"/>
+      <c r="H21" s="123"/>
+      <c r="I21" s="123"/>
     </row>
     <row r="22" spans="1:18" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="146" t="str">
+      <c r="A22" s="145" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2024 Schedule
 (as of 1-24-2024, subject to change)</v>
       </c>
-      <c r="B22" s="147"/>
-      <c r="C22" s="147"/>
-      <c r="D22" s="147"/>
-      <c r="E22" s="147"/>
-      <c r="F22" s="147"/>
-      <c r="G22" s="147"/>
-      <c r="H22" s="147"/>
-      <c r="I22" s="148"/>
+      <c r="B22" s="146"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="146"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="146"/>
+      <c r="H22" s="146"/>
+      <c r="I22" s="147"/>
     </row>
     <row r="23" spans="1:18" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="str">
@@ -2641,11 +2647,11 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="149">
+      <c r="A24" s="148">
         <f>A15-1</f>
         <v>8</v>
       </c>
-      <c r="B24" s="135" t="s">
+      <c r="B24" s="134" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="98">
@@ -2676,24 +2682,24 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="L24" s="124"/>
-      <c r="M24" s="122"/>
-      <c r="N24" s="122"/>
-      <c r="O24" s="122"/>
-      <c r="P24" s="122"/>
-      <c r="Q24" s="122"/>
-      <c r="R24" s="122"/>
+      <c r="L24" s="123"/>
+      <c r="M24" s="121"/>
+      <c r="N24" s="121"/>
+      <c r="O24" s="121"/>
+      <c r="P24" s="121"/>
+      <c r="Q24" s="121"/>
+      <c r="R24" s="121"/>
     </row>
     <row r="25" spans="1:18" ht="102.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="142"/>
-      <c r="B25" s="135"/>
+      <c r="A25" s="141"/>
+      <c r="B25" s="134"/>
       <c r="C25" s="53"/>
       <c r="D25" s="22" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="s">
@@ -2701,19 +2707,19 @@
       </c>
       <c r="I25" s="36"/>
       <c r="L25" s="25"/>
-      <c r="M25" s="122"/>
-      <c r="N25" s="122"/>
-      <c r="O25" s="122"/>
-      <c r="P25" s="122"/>
-      <c r="Q25" s="122"/>
+      <c r="M25" s="121"/>
+      <c r="N25" s="121"/>
+      <c r="O25" s="121"/>
+      <c r="P25" s="121"/>
+      <c r="Q25" s="121"/>
       <c r="R25" s="25"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="142">
+      <c r="A26" s="141">
         <f>A24 - 1</f>
         <v>7</v>
       </c>
-      <c r="B26" s="135"/>
+      <c r="B26" s="134"/>
       <c r="C26" s="7">
         <f>I24 + 1</f>
         <v>17</v>
@@ -2742,50 +2748,50 @@
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="L26" s="122"/>
-      <c r="M26" s="122"/>
-      <c r="N26" s="122"/>
-      <c r="O26" s="122"/>
-      <c r="P26" s="122"/>
-      <c r="Q26" s="122"/>
-      <c r="R26" s="122"/>
+      <c r="L26" s="121"/>
+      <c r="M26" s="121"/>
+      <c r="N26" s="121"/>
+      <c r="O26" s="121"/>
+      <c r="P26" s="121"/>
+      <c r="Q26" s="121"/>
+      <c r="R26" s="121"/>
     </row>
     <row r="27" spans="1:18" ht="129.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="142"/>
-      <c r="B27" s="135"/>
-      <c r="C27" s="121"/>
+      <c r="A27" s="141"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="120"/>
       <c r="D27" s="26" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="114" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F27" s="57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" s="114" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="I27" s="120" t="s">
-        <v>53</v>
-      </c>
       <c r="L27" s="25"/>
-      <c r="M27" s="122"/>
-      <c r="N27" s="124"/>
-      <c r="O27" s="122"/>
-      <c r="P27" s="124"/>
-      <c r="Q27" s="122"/>
+      <c r="M27" s="121"/>
+      <c r="N27" s="123"/>
+      <c r="O27" s="121"/>
+      <c r="P27" s="123"/>
+      <c r="Q27" s="121"/>
       <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="142">
+      <c r="A28" s="141">
         <f>A26 - 1</f>
         <v>6</v>
       </c>
-      <c r="B28" s="135"/>
+      <c r="B28" s="134"/>
       <c r="C28" s="7">
         <f>I26 + 1</f>
         <v>24</v>
@@ -2814,48 +2820,48 @@
         <f t="shared" ref="I28" si="9">H28 + 1</f>
         <v>30</v>
       </c>
-      <c r="L28" s="122"/>
-      <c r="M28" s="122"/>
-      <c r="N28" s="122"/>
-      <c r="O28" s="122"/>
-      <c r="P28" s="122"/>
-      <c r="Q28" s="122"/>
-      <c r="R28" s="122"/>
+      <c r="L28" s="121"/>
+      <c r="M28" s="121"/>
+      <c r="N28" s="121"/>
+      <c r="O28" s="121"/>
+      <c r="P28" s="121"/>
+      <c r="Q28" s="121"/>
+      <c r="R28" s="121"/>
     </row>
     <row r="29" spans="1:18" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="139"/>
-      <c r="B29" s="134"/>
+      <c r="A29" s="138"/>
+      <c r="B29" s="133"/>
       <c r="C29" s="115"/>
       <c r="D29" s="23" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G29" s="99"/>
       <c r="H29" s="74" t="s">
-        <v>48</v>
-      </c>
-      <c r="I29" s="119" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="I29" s="118" t="s">
+        <v>47</v>
       </c>
       <c r="L29" s="25"/>
-      <c r="M29" s="122"/>
+      <c r="M29" s="121"/>
       <c r="N29" s="25"/>
-      <c r="O29" s="122"/>
+      <c r="O29" s="121"/>
       <c r="P29" s="25"/>
-      <c r="Q29" s="124"/>
+      <c r="Q29" s="123"/>
       <c r="R29" s="25"/>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="143">
+      <c r="A30" s="142">
         <f>A28 -1</f>
         <v>5</v>
       </c>
-      <c r="B30" s="131" t="s">
+      <c r="B30" s="130" t="s">
         <v>43</v>
       </c>
       <c r="C30" s="105">
@@ -2887,30 +2893,32 @@
       </c>
     </row>
     <row r="31" spans="1:18" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="144"/>
-      <c r="B31" s="130"/>
-      <c r="C31" s="118" t="s">
-        <v>66</v>
+      <c r="A31" s="143"/>
+      <c r="B31" s="129"/>
+      <c r="C31" s="153" t="s">
+        <v>47</v>
       </c>
       <c r="D31" s="107" t="s">
-        <v>48</v>
-      </c>
-      <c r="E31" s="27"/>
+        <v>47</v>
+      </c>
+      <c r="E31" s="52" t="s">
+        <v>65</v>
+      </c>
       <c r="F31" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G31" s="81"/>
       <c r="H31" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I31" s="28"/>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="145">
+      <c r="A32" s="144">
         <f>A30 -1</f>
         <v>4</v>
       </c>
-      <c r="B32" s="131" t="s">
+      <c r="B32" s="130" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="62">
@@ -2943,30 +2951,30 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="93" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="136"/>
-      <c r="B33" s="132"/>
+      <c r="A33" s="135"/>
+      <c r="B33" s="131"/>
       <c r="C33" s="29"/>
       <c r="D33" s="116" t="s">
         <v>28</v>
       </c>
       <c r="E33" s="117" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G33" s="27"/>
       <c r="H33" s="109" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I33" s="28"/>
     </row>
     <row r="34" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="136">
+      <c r="A34" s="135">
         <f>A32 -1</f>
         <v>3</v>
       </c>
-      <c r="B34" s="132"/>
+      <c r="B34" s="131"/>
       <c r="C34" s="27">
         <f>I32 + 1</f>
         <v>14</v>
@@ -2997,8 +3005,8 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="136"/>
-      <c r="B35" s="132"/>
+      <c r="A35" s="135"/>
+      <c r="B35" s="131"/>
       <c r="C35" s="29"/>
       <c r="D35" s="108" t="s">
         <v>6</v>
@@ -3014,11 +3022,11 @@
       <c r="I35" s="28"/>
     </row>
     <row r="36" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="136">
+      <c r="A36" s="135">
         <f>A34 -1</f>
         <v>2</v>
       </c>
-      <c r="B36" s="132"/>
+      <c r="B36" s="131"/>
       <c r="C36" s="29">
         <f>I34 + 1</f>
         <v>21</v>
@@ -3049,8 +3057,8 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="64.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="137"/>
-      <c r="B37" s="130"/>
+      <c r="A37" s="136"/>
+      <c r="B37" s="129"/>
       <c r="C37" s="60"/>
       <c r="D37" s="44" t="s">
         <v>25</v>
@@ -3066,11 +3074,11 @@
       <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="138">
+      <c r="A38" s="137">
         <f>A36 -1</f>
         <v>1</v>
       </c>
-      <c r="B38" s="133" t="s">
+      <c r="B38" s="132" t="s">
         <v>44</v>
       </c>
       <c r="C38" s="17">
@@ -3102,8 +3110,8 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="139"/>
-      <c r="B39" s="134"/>
+      <c r="A39" s="138"/>
+      <c r="B39" s="133"/>
       <c r="C39" s="102"/>
       <c r="D39" s="50" t="s">
         <v>6</v>
@@ -3117,14 +3125,14 @@
         <v>38</v>
       </c>
       <c r="I39" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="140" t="s">
+      <c r="A40" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="135" t="s">
+      <c r="B40" s="134" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="20">
@@ -3157,17 +3165,17 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="134.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="141"/>
-      <c r="B41" s="134"/>
+      <c r="A41" s="140"/>
+      <c r="B41" s="133"/>
       <c r="C41" s="63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E41" s="64"/>
       <c r="F41" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G41" s="21"/>
       <c r="H41" s="78"/>

</xml_diff>